<commit_message>
Ok per la serata al PBG
</commit_message>
<xml_diff>
--- a/notebook/dataset.xlsx
+++ b/notebook/dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,42 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t xml:space="preserve">user_AskProv</t>
   </si>
   <si>
-    <t xml:space="preserve">Quante fattorie didattiche ci sono in provincia di [PROVINCIA](Salerno)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche in provincia di [PROVINCIA](Salerno)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli)?</t>
+    <t xml:space="preserve">Quante fattorie didattiche ci sono in provincia di [PROVINCIA](Salerno) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ci sono fattorie didattiche in provincia di [PROVINCIA](Salerno) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli) ?</t>
   </si>
   <si>
     <t xml:space="preserve">user_AskCity</t>
   </si>
   <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche ad [SEDE](Eboli)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quante fattorie didattiche ci sono a [SEDE](Salerno)?</t>
+    <t xml:space="preserve">Ci sono fattorie didattiche ad [SEDE](Eboli) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quante fattorie didattiche ci sono a [SEDE](Salerno) ?</t>
   </si>
   <si>
     <t xml:space="preserve">user_AskProvWithParams</t>
   </si>
   <si>
-    <t xml:space="preserve">Quante fattorie didattiche ci sono in provincia di [PROVINCIA](Salerno) con [categoria](allevamento)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche in provincia di [PROVINCIA](Salerno) con produzione di [CATEGORIA](formaggi)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli) che producono [CATEGORIA](formaggi)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli) con coltivazione di [CATEGORIA](frutta)?</t>
+    <t xml:space="preserve">Quante fattorie didattiche ci sono in provincia di [PROVINCIA](Salerno) con [categoria](allevamento) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ci sono fattorie didattiche in provincia di [PROVINCIA](Salerno) con produzione di [CATEGORIA](formaggi) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli) che producono [CATEGORIA](formaggi) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ci sono fattorie didattiche nella provincia di [PROVINCIA](Napoli) con coltivazione di [CATEGORIA](frutta) ?</t>
   </si>
   <si>
     <t xml:space="preserve">bot_ReplyProv</t>
@@ -169,6 +169,36 @@
   </si>
   <si>
     <t xml:space="preserve">MONTECORVINO PUGLIANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALVI RISORTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIANO DI SORRENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIGLIANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCOLISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SESSA AURUNCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASCEA MARINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIGNATARO MAGGIORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASTELNUOVO CILENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASTEL CAMPAGNANO</t>
   </si>
 </sst>
 </file>
@@ -243,13 +273,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -271,11 +305,11 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.28"/>
@@ -357,7 +391,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.32"/>
@@ -410,7 +444,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.61"/>
   </cols>
@@ -464,13 +498,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.19"/>
@@ -615,6 +649,59 @@
       <c r="A22" s="0" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -638,7 +725,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -661,7 +748,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.31"/>

</xml_diff>